<commit_message>
Atualização automática de TAQUARI.xlsx
</commit_message>
<xml_diff>
--- a/TAQUARI.xlsx
+++ b/TAQUARI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E7BDCE4-2C8E-4BCD-9BA4-E235BCF7742D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{270C8B5C-5705-4AAA-A124-A461A2164E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1289,7 +1289,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{B7D3A971-DBD5-46D4-AC1B-EA63BE1824BF}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{AEC19959-C2EE-42EB-9D56-99908B25ED7C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1319,10 +1319,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C12ECB37-48E4-4D44-AA9F-FE073EF9FCB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C252CFD4-F0DC-4C94-BDEF-F2A250F57FC3}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1360,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F659A99D-DC75-4ACF-BA58-964D6574330C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F28AA022-DAED-48C0-A4C6-04A17E82DB24}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1423,7 +1423,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAFD8044-F34A-4ECC-B9B5-273391FA0DBC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D0E12BF-E52B-45A6-B475-C9E44099831B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1442,7 +1442,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{271DB805-6AB5-CA69-7F41-6C29BC17660B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ADAA596-0FDD-FF32-7489-4240738C1EBF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1491,7 +1491,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AFB8935-5AD2-9BAA-C102-DE5A4774FFAD}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0B4D0CF-BADB-F46C-CBBF-3F6BFD785B67}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1510,7 +1510,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F98771B9-B505-C113-8A3D-0AD480D9F4A1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FD270B4-BD0C-30DF-93DF-FB52478D9D89}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1541,7 +1541,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC853236-E656-049B-2F37-0E80DFBFA62A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C7A4FF8-E4EE-DA28-C0D4-0A4B400495CF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1572,7 +1572,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74B3629F-E451-D5D7-D3F8-D904B8793C76}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C67A4FDD-7806-2247-7A9C-354B9A3E27F8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1615,7 +1615,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B78FED5-5613-4D55-80B4-323D6ACBF2B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6C8E02A-7865-4BEC-A315-0EC6F724F7F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1653,7 +1653,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577C3652-FCC6-462A-A35B-8C66F05FCCB6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D48F630-4C21-4A17-8380-B31FAB920D10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1696,7 +1696,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F1CA66B-7E64-4ACA-B805-5F65DDAF000E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4323A61C-D77C-4F59-8E61-F115F7A3BBA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2009,7 +2009,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A492AB9-CB19-4D2A-905E-FBDCF4FABE57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D095100B-9DFA-4BA4-8452-BDD76EC16C65}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>